<commit_message>
singe Map Move able
</commit_message>
<xml_diff>
--- a/데이터베이스_외부.xlsx
+++ b/데이터베이스_외부.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\정성진\Desktop\학교\maze of memorries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\정성진\Desktop\school\maze of memorries\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" tabRatio="697"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" tabRatio="697" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="계정" sheetId="1" r:id="rId1"/>
@@ -523,10 +523,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>STAGE_INFO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>NUMBER</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -711,10 +707,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MAP_INFO_5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>int(4)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -731,10 +723,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MAP_INFO_7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>5+5-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -784,6 +772,18 @@
   </si>
   <si>
     <t>별 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SINGLE_MAP_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MULTI_MAP_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MULTI_MAP_7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1152,7 +1152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1296,13 +1296,14 @@
   <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="4" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
@@ -1310,7 +1311,7 @@
         <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
@@ -1319,7 +1320,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>120</v>
@@ -1327,14 +1328,14 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1348,15 +1349,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="29.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
@@ -1364,7 +1365,7 @@
         <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
@@ -1373,7 +1374,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>120</v>
@@ -1385,10 +1386,10 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1402,7 +1403,7 @@
   <dimension ref="B2:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1507,7 +1508,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>65</v>
@@ -1532,14 +1533,14 @@
   <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
@@ -1547,7 +1548,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>122</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -1558,7 +1559,7 @@
         <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -1569,7 +1570,7 @@
         <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -1580,7 +1581,7 @@
         <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -1591,7 +1592,7 @@
         <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -1599,10 +1600,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -1613,10 +1614,10 @@
         <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1646,18 +1647,18 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
@@ -1668,7 +1669,7 @@
         <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -1679,7 +1680,7 @@
         <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -1690,7 +1691,7 @@
         <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
@@ -1701,7 +1702,7 @@
         <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1731,7 +1732,7 @@
         <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -1759,7 +1760,7 @@
         <v>86</v>
       </c>
       <c r="F5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -1773,7 +1774,7 @@
         <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -1787,7 +1788,7 @@
         <v>72</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -1801,7 +1802,7 @@
         <v>72</v>
       </c>
       <c r="F8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -1809,13 +1810,13 @@
         <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2003,12 +2004,12 @@
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C10" t="s">
         <v>104</v>
@@ -2016,7 +2017,7 @@
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C11" t="s">
         <v>104</v>
@@ -2024,7 +2025,7 @@
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" t="s">
         <v>65</v>
@@ -2060,7 +2061,7 @@
         <v>87</v>
       </c>
       <c r="L2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2068,28 +2069,28 @@
         <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" t="s">
+        <v>151</v>
+      </c>
+      <c r="L4" t="s">
         <v>150</v>
-      </c>
-      <c r="J4" t="s">
-        <v>152</v>
-      </c>
-      <c r="L4" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -2118,7 +2119,7 @@
         <v>105</v>
       </c>
       <c r="L5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2147,12 +2148,12 @@
         <v>105</v>
       </c>
       <c r="L6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>96</v>
@@ -2179,7 +2180,7 @@
         <v>105</v>
       </c>
       <c r="L7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2208,7 +2209,7 @@
         <v>105</v>
       </c>
       <c r="L8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -2237,7 +2238,7 @@
         <v>105</v>
       </c>
       <c r="L9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2266,12 +2267,12 @@
         <v>105</v>
       </c>
       <c r="L10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>100</v>
@@ -2298,7 +2299,7 @@
         <v>105</v>
       </c>
       <c r="L11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -2327,7 +2328,7 @@
         <v>105</v>
       </c>
       <c r="L12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2356,7 +2357,7 @@
         <v>59</v>
       </c>
       <c r="L13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -2385,7 +2386,7 @@
         <v>59</v>
       </c>
       <c r="L14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2415,12 +2416,12 @@
         <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C4" s="3">
         <v>5</v>
@@ -2430,10 +2431,10 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -2444,14 +2445,14 @@
         <v>39</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
         <v>65</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -2459,22 +2460,22 @@
         <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
         <v>65</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" s="3">
         <v>60</v>
@@ -2484,10 +2485,10 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
scroll & game clear imprement
</commit_message>
<xml_diff>
--- a/데이터베이스_외부.xlsx
+++ b/데이터베이스_외부.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="198">
   <si>
     <t>계정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -808,6 +808,22 @@
   </si>
   <si>
     <t>크기 100으로 변경, 이름_번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1206,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1826,10 +1842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G8"/>
+  <dimension ref="B2:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1840,7 +1856,7 @@
     <col min="6" max="6" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1848,7 +1864,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1862,7 +1878,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1874,7 +1890,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>183</v>
       </c>
@@ -1885,8 +1901,11 @@
       <c r="F6" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>190</v>
       </c>
@@ -1900,8 +1919,11 @@
       <c r="G7" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
     </row>
   </sheetData>
@@ -2019,10 +2041,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F9"/>
+  <dimension ref="A2:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2033,7 +2055,7 @@
     <col min="6" max="6" width="17.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>21</v>
       </c>
@@ -2041,7 +2063,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
@@ -2055,7 +2077,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>196</v>
+      </c>
       <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
@@ -2070,7 +2095,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
@@ -2084,7 +2109,10 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>197</v>
+      </c>
       <c r="B7" s="6" t="s">
         <v>25</v>
       </c>
@@ -2099,7 +2127,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
@@ -2113,7 +2141,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>27</v>
       </c>

</xml_diff>